<commit_message>
implement withdraw and wallet-topup
</commit_message>
<xml_diff>
--- a/docs/feature-design.xlsx
+++ b/docs/feature-design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="9" r:id="rId1"/>
@@ -18,16 +18,11 @@
     <sheet name="bank" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="225">
   <si>
     <t>Xây dựng 1 service  quản lí người dùng:</t>
   </si>
@@ -2763,8 +2758,8 @@
   </sheetPr>
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3798,10 +3793,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4080,63 +4075,63 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="A49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" t="s">
-        <v>41</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" t="s">
-        <v>64</v>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>146</v>
+      <c r="A54" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>145</v>
+        <v>10</v>
+      </c>
+      <c r="C55" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>35</v>
-      </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C56" t="s">
         <v>37</v>
@@ -4144,33 +4139,25 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="C57" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>59</v>
-      </c>
-      <c r="C58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A58" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="59" spans="1:4" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
         <v>40</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C59" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D59" s="5" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add websocket for changed balance of wallet envet
</commit_message>
<xml_diff>
--- a/docs/feature-design.xlsx
+++ b/docs/feature-design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="9" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="236">
   <si>
     <t>Xây dựng 1 service  quản lí người dùng:</t>
   </si>
@@ -415,12 +415,6 @@
   </si>
   <si>
     <t>Chanel name</t>
-  </si>
-  <si>
-    <t>UPDATE_WALLET</t>
-  </si>
-  <si>
-    <t>Send data</t>
   </si>
   <si>
     <t xml:space="preserve">Xây dựng hệ thống cho phép người dùng cash-in/ cash-out </t>
@@ -727,6 +721,24 @@
   </si>
   <si>
     <t>bankname</t>
+  </si>
+  <si>
+    <t>/ws/topic/updated_wallet</t>
+  </si>
+  <si>
+    <t>Endpoint</t>
+  </si>
+  <si>
+    <t>/ws-stomp</t>
+  </si>
+  <si>
+    <t>{"userid":"1584784717714","balance":91159792}</t>
+  </si>
+  <si>
+    <t>Receive data</t>
+  </si>
+  <si>
+    <t>Sample Receive Data</t>
   </si>
 </sst>
 </file>
@@ -2640,7 +2652,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2688,7 +2700,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2696,7 +2708,7 @@
         <v>33</v>
       </c>
       <c r="B61" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2877,7 +2889,7 @@
         <v>80</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2999,7 +3011,7 @@
         <v>41</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3020,14 +3032,14 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C30" t="s">
         <v>41</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3181,7 +3193,7 @@
   </sheetPr>
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -3240,7 +3252,7 @@
         <v>14</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3269,12 +3281,12 @@
         <v>1</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3358,7 +3370,7 @@
     </row>
     <row r="20" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C20" t="s">
         <v>41</v>
@@ -3438,12 +3450,12 @@
         <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C32" t="s">
         <v>41</v>
@@ -3462,7 +3474,7 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3521,7 +3533,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3529,7 +3541,7 @@
         <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3548,7 +3560,7 @@
         <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D48" t="s">
         <v>87</v>
@@ -3567,7 +3579,7 @@
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D50" t="s">
         <v>37</v>
@@ -3588,16 +3600,16 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="19.109375" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
   </cols>
@@ -3779,88 +3791,104 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="B35" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="B35" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="B36" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>10</v>
       </c>
-      <c r="C38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>115</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>235</v>
+      </c>
+      <c r="B42" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>10</v>
       </c>
-      <c r="C43" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="50" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>40</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C50" t="s">
         <v>41</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D50" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>57</v>
       </c>
-      <c r="C47" t="s">
-        <v>176</v>
+      <c r="C51" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3890,7 +3918,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3900,7 +3928,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3908,16 +3936,16 @@
         <v>61</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>135</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3939,7 +3967,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3961,7 +3989,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C11">
         <v>561278</v>
@@ -3978,7 +4006,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3991,7 +4019,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C15">
         <v>200000</v>
@@ -4004,7 +4032,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4012,7 +4040,7 @@
         <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4084,7 +4112,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4092,7 +4120,7 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4127,12 +4155,12 @@
         <v>41</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4140,7 +4168,7 @@
         <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4188,7 +4216,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4196,7 +4224,7 @@
         <v>33</v>
       </c>
       <c r="B54" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4239,7 +4267,7 @@
         <v>41</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -4274,12 +4302,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4290,18 +4318,18 @@
         <v>57</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B5">
         <v>200000</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4311,7 +4339,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4322,7 +4350,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -4342,7 +4370,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C12" t="s">
         <v>37</v>
@@ -4382,7 +4410,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4390,7 +4418,7 @@
         <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4425,7 +4453,7 @@
         <v>41</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -4462,7 +4490,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4472,18 +4500,18 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>153</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>155</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>50</v>
@@ -4497,16 +4525,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="E6" s="14" t="s">
         <v>157</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>159</v>
       </c>
       <c r="F6" s="12">
         <v>1</v>
@@ -4517,12 +4545,12 @@
     </row>
     <row r="7" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="F7" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -4534,7 +4562,7 @@
         <v>57</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>12</v>
@@ -4543,16 +4571,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C10">
         <v>200000</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F10" s="10"/>
     </row>
@@ -4563,7 +4591,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4571,7 +4599,7 @@
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4593,7 +4621,7 @@
         <v>64</v>
       </c>
       <c r="D17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4606,13 +4634,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C19" t="s">
         <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,7 +4669,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4649,7 +4677,7 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4684,12 +4712,12 @@
         <v>41</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C32" t="s">
         <v>37</v>
@@ -4697,7 +4725,7 @@
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -4737,12 +4765,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4752,7 +4780,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4760,7 +4788,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>16</v>
@@ -4774,29 +4802,29 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" t="s">
         <v>185</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="E7" t="s">
         <v>186</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="E7" t="s">
-        <v>188</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4804,51 +4832,51 @@
         <v>17</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>115</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>49</v>
@@ -4856,7 +4884,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C15">
         <v>100000</v>
@@ -4870,18 +4898,18 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>96</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>14</v>
@@ -4889,13 +4917,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -4903,10 +4931,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -4916,10 +4944,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -4927,7 +4955,7 @@
         <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -4935,7 +4963,7 @@
         <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C26" t="s">
         <v>37</v>
@@ -4943,7 +4971,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C27" t="s">
         <v>37</v>
@@ -4978,15 +5006,15 @@
         <v>41</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B33" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4994,7 +5022,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5002,7 +5030,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C35" t="s">
         <v>37</v>
@@ -5045,12 +5073,12 @@
         <v>41</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C42" t="s">
         <v>37</v>
@@ -5059,10 +5087,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B44" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -5070,7 +5098,7 @@
         <v>33</v>
       </c>
       <c r="B45" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -5078,7 +5106,7 @@
         <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C46" t="s">
         <v>37</v>
@@ -5086,7 +5114,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C47" t="s">
         <v>37</v>
@@ -5121,12 +5149,12 @@
         <v>41</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -5134,7 +5162,7 @@
         <v>33</v>
       </c>
       <c r="B54" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -5142,7 +5170,7 @@
         <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C55" t="s">
         <v>37</v>
@@ -5150,7 +5178,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C56" t="s">
         <v>37</v>
@@ -5185,12 +5213,12 @@
         <v>41</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -5198,7 +5226,7 @@
         <v>33</v>
       </c>
       <c r="B64" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -5206,7 +5234,7 @@
         <v>35</v>
       </c>
       <c r="B65" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C65" t="s">
         <v>37</v>
@@ -5214,7 +5242,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C66" t="s">
         <v>37</v>
@@ -5249,7 +5277,7 @@
         <v>41</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>